<commit_message>
Filling up folder with stuff to include with manuscript submission
</commit_message>
<xml_diff>
--- a/Supplemental/assembly_stats.xlsx
+++ b/Supplemental/assembly_stats.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Supplemental\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF92612-CAFD-4980-BBA9-E9BBD91CB500}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{5E0D713C-FBC2-4676-9850-D9313BB3C08D}"/>
   </bookViews>
@@ -15,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="96">
   <si>
     <t>Lake Mendota</t>
   </si>
@@ -36,9 +37,6 @@
     <t>Trout Bog Hypolimnion</t>
   </si>
   <si>
-    <t># Samples</t>
-  </si>
-  <si>
     <t>Time span</t>
   </si>
   <si>
@@ -52,9 +50,6 @@
   </si>
   <si>
     <t># of curated genomes</t>
-  </si>
-  <si>
-    <t>Total base pairs</t>
   </si>
   <si>
     <t>agenome</t>
@@ -330,26 +325,26 @@
     <t>Jun. 2008 - Nov. 2012</t>
   </si>
   <si>
-    <t>1.26x10^11</t>
-  </si>
-  <si>
-    <t>6.72x10^10</t>
-  </si>
-  <si>
     <t>May 2007 - Aug.2009</t>
   </si>
   <si>
-    <t>7.18x10^10</t>
-  </si>
-  <si>
     <t>Assembly information</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t># Pooled Samples</t>
+  </si>
+  <si>
+    <t>IMGOID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +382,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -425,6 +427,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4691,78 +4694,81 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="7">
+        <v>3300002835</v>
+      </c>
+      <c r="C3">
+        <v>3300000439</v>
+      </c>
+      <c r="D3">
+        <v>3300000553</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>94</v>
-      </c>
-      <c r="C4">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>45</v>
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>93</v>
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" s="2">
         <v>3368129613</v>
@@ -4776,7 +4782,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>9912431</v>
@@ -4790,7 +4796,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>18675</v>
@@ -4804,7 +4810,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>230906243</v>
@@ -4818,7 +4824,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>99</v>
@@ -4832,6 +4838,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4852,25 +4859,25 @@
   <sheetData>
     <row r="1" spans="1:12" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G1" s="3">
         <v>3300002296</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I1" s="3">
         <v>413144446</v>
@@ -4886,25 +4893,25 @@
     <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G2" s="3">
         <v>3300002294</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3">
         <v>517462778</v>
@@ -4916,25 +4923,25 @@
     <row r="3" spans="1:12" ht="375" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="3">
         <v>3300002350</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3">
         <v>548374342</v>
@@ -4946,25 +4953,25 @@
     <row r="4" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G4" s="3">
         <v>3300002370</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I4" s="3">
         <v>533631939</v>
@@ -4976,25 +4983,25 @@
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G5" s="3">
         <v>3300002278</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I5" s="3">
         <v>374467379</v>
@@ -5006,25 +5013,25 @@
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G6" s="3">
         <v>3300002390</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="3">
         <v>653328173</v>
@@ -5036,25 +5043,25 @@
     <row r="7" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G7" s="3">
         <v>3300002363</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I7" s="3">
         <v>424807098</v>
@@ -5066,25 +5073,25 @@
     <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G8" s="3">
         <v>3300002368</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I8" s="3">
         <v>449325882</v>
@@ -5096,25 +5103,25 @@
     <row r="9" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G9" s="3">
         <v>3300002302</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3">
         <v>404215834</v>
@@ -5126,25 +5133,25 @@
     <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G10" s="3">
         <v>3300002367</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I10" s="3">
         <v>441114359</v>
@@ -5156,25 +5163,25 @@
     <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G11" s="3">
         <v>3300002394</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I11" s="3">
         <v>591324053</v>
@@ -5186,25 +5193,25 @@
     <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G12" s="3">
         <v>3300002297</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I12" s="3">
         <v>448285939</v>
@@ -5216,25 +5223,25 @@
     <row r="13" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G13" s="3">
         <v>3300002272</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I13" s="3">
         <v>597297025</v>
@@ -5246,25 +5253,25 @@
     <row r="14" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G14" s="3">
         <v>3300002395</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I14" s="3">
         <v>630077326</v>
@@ -5276,25 +5283,25 @@
     <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G15" s="3">
         <v>3300002273</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I15" s="3">
         <v>457861846</v>
@@ -5306,25 +5313,25 @@
     <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G16" s="3">
         <v>3300002269</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I16" s="3">
         <v>475196717</v>
@@ -5336,25 +5343,25 @@
     <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G17" s="3">
         <v>3300002371</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I17" s="3">
         <v>471465802</v>
@@ -5366,25 +5373,25 @@
     <row r="18" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G18" s="3">
         <v>3300002304</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I18" s="3">
         <v>462874933</v>
@@ -5396,25 +5403,25 @@
     <row r="19" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G19" s="3">
         <v>3300002403</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I19" s="3">
         <v>1009461251</v>
@@ -5426,25 +5433,25 @@
     <row r="20" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G20" s="3">
         <v>3300002279</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I20" s="3">
         <v>1064069462</v>
@@ -5456,25 +5463,25 @@
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G21" s="3">
         <v>3300002396</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I21" s="3">
         <v>621286104</v>
@@ -5486,25 +5493,25 @@
     <row r="22" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G22" s="3">
         <v>3300002381</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I22" s="3">
         <v>514383084</v>
@@ -5516,25 +5523,25 @@
     <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G23" s="3">
         <v>3300002404</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I23" s="3">
         <v>1325913298</v>
@@ -5546,25 +5553,25 @@
     <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G24" s="3">
         <v>3300002398</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I24" s="3">
         <v>880947503</v>
@@ -5576,25 +5583,25 @@
     <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G25" s="3">
         <v>3300002362</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I25" s="3">
         <v>420539664</v>
@@ -5606,25 +5613,25 @@
     <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G26" s="3">
         <v>3300002402</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I26" s="3">
         <v>1019675415</v>
@@ -5636,25 +5643,25 @@
     <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G27" s="3">
         <v>3300002276</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I27" s="3">
         <v>735681494</v>
@@ -5666,25 +5673,25 @@
     <row r="28" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G28" s="3">
         <v>3300002385</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I28" s="3">
         <v>528486780</v>
@@ -5696,25 +5703,25 @@
     <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G29" s="3">
         <v>3300002369</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I29" s="3">
         <v>482931200</v>
@@ -5726,25 +5733,25 @@
     <row r="30" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G30" s="3">
         <v>3300002277</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I30" s="3">
         <v>271813930</v>
@@ -5756,25 +5763,25 @@
     <row r="31" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G31" s="3">
         <v>3300002389</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I31" s="3">
         <v>576260407</v>
@@ -5786,25 +5793,25 @@
     <row r="32" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G32" s="3">
         <v>3300002372</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I32" s="3">
         <v>492295187</v>
@@ -5816,25 +5823,25 @@
     <row r="33" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G33" s="3">
         <v>3300002380</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I33" s="3">
         <v>495361996</v>
@@ -5846,25 +5853,25 @@
     <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G34" s="3">
         <v>3300002365</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I34" s="3">
         <v>490265277</v>
@@ -5876,25 +5883,25 @@
     <row r="35" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G35" s="3">
         <v>3300002306</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I35" s="3">
         <v>610458864</v>
@@ -5906,25 +5913,25 @@
     <row r="36" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G36" s="3">
         <v>3300002349</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I36" s="3">
         <v>430387461</v>
@@ -5936,25 +5943,25 @@
     <row r="37" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G37" s="3">
         <v>3300002361</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I37" s="3">
         <v>431209578</v>
@@ -5966,25 +5973,25 @@
     <row r="38" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G38" s="3">
         <v>3300002384</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I38" s="3">
         <v>512915657</v>
@@ -5996,25 +6003,25 @@
     <row r="39" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G39" s="3">
         <v>3300002348</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I39" s="3">
         <v>286483067</v>
@@ -6026,25 +6033,25 @@
     <row r="40" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G40" s="3">
         <v>3300002386</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I40" s="3">
         <v>522635300</v>
@@ -6056,25 +6063,25 @@
     <row r="41" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G41" s="3">
         <v>3300002373</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I41" s="3">
         <v>528504942</v>
@@ -6086,25 +6093,25 @@
     <row r="42" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G42" s="3">
         <v>3300002383</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I42" s="3">
         <v>510100120</v>
@@ -6116,25 +6123,25 @@
     <row r="43" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G43" s="3">
         <v>3300002399</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I43" s="3">
         <v>920981029</v>
@@ -6146,25 +6153,25 @@
     <row r="44" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G44" s="3">
         <v>3300002353</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I44" s="3">
         <v>304911884</v>
@@ -6176,25 +6183,25 @@
     <row r="45" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G45" s="3">
         <v>3300002379</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I45" s="3">
         <v>533551478</v>
@@ -6206,25 +6213,25 @@
     <row r="46" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G46" s="3">
         <v>3300002271</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I46" s="3">
         <v>494030836</v>
@@ -6236,25 +6243,25 @@
     <row r="47" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G47" s="3">
         <v>3300002354</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I47" s="3">
         <v>347426642</v>
@@ -6266,25 +6273,25 @@
     <row r="48" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G48" s="3">
         <v>3300002401</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I48" s="3">
         <v>1038574287</v>
@@ -6296,25 +6303,25 @@
     <row r="49" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G49" s="3">
         <v>3300002364</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I49" s="3">
         <v>456704697</v>
@@ -6326,25 +6333,25 @@
     <row r="50" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G50" s="3">
         <v>3300002355</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I50" s="3">
         <v>395099976</v>
@@ -6356,25 +6363,25 @@
     <row r="51" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G51" s="3">
         <v>3300002382</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I51" s="3">
         <v>513593012</v>
@@ -6386,25 +6393,25 @@
     <row r="52" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G52" s="3">
         <v>3300002275</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I52" s="3">
         <v>612556446</v>
@@ -6416,25 +6423,25 @@
     <row r="53" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G53" s="3">
         <v>3300002375</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I53" s="3">
         <v>482459367</v>
@@ -6446,25 +6453,25 @@
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G54" s="3">
         <v>3300002270</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I54" s="3">
         <v>490914275</v>
@@ -6476,25 +6483,25 @@
     <row r="55" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G55" s="3">
         <v>3300002374</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I55" s="3">
         <v>481294843</v>
@@ -6506,25 +6513,25 @@
     <row r="56" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G56" s="3">
         <v>3300002305</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I56" s="3">
         <v>495591861</v>
@@ -6536,25 +6543,25 @@
     <row r="57" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G57" s="3">
         <v>3300002299</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I57" s="3">
         <v>383623834</v>
@@ -6566,25 +6573,25 @@
     <row r="58" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G58" s="3">
         <v>3300002388</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I58" s="3">
         <v>590103659</v>
@@ -6596,25 +6603,25 @@
     <row r="59" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G59" s="3">
         <v>3300002400</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I59" s="3">
         <v>875791028</v>
@@ -6626,25 +6633,25 @@
     <row r="60" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G60" s="3">
         <v>3300002360</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I60" s="3">
         <v>423066712</v>
@@ -6656,25 +6663,25 @@
     <row r="61" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G61" s="3">
         <v>3300002358</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I61" s="3">
         <v>400203454</v>
@@ -6686,25 +6693,25 @@
     <row r="62" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G62" s="3">
         <v>3300002366</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I62" s="3">
         <v>315138119</v>
@@ -6716,25 +6723,25 @@
     <row r="63" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G63" s="3">
         <v>3300002408</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I63" s="3">
         <v>0</v>
@@ -6746,25 +6753,25 @@
     <row r="64" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D64" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G64" s="3">
         <v>3300002274</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I64" s="3">
         <v>536639168</v>
@@ -6776,25 +6783,25 @@
     <row r="65" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D65" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F65" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G65" s="3">
         <v>3300002393</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I65" s="3">
         <v>572730848</v>
@@ -6806,25 +6813,25 @@
     <row r="66" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D66" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G66" s="3">
         <v>3300002356</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I66" s="3">
         <v>372717908</v>
@@ -6836,25 +6843,25 @@
     <row r="67" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G67" s="3">
         <v>3300002295</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I67" s="3">
         <v>414544282</v>
@@ -6866,25 +6873,25 @@
     <row r="68" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D68" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G68" s="3">
         <v>3300002300</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I68" s="3">
         <v>382271149</v>
@@ -6896,25 +6903,25 @@
     <row r="69" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D69" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F69" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G69" s="3">
         <v>3300002303</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I69" s="3">
         <v>407802015</v>
@@ -6926,25 +6933,25 @@
     <row r="70" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D70" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F70" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G70" s="3">
         <v>3300002397</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I70" s="3">
         <v>827713149</v>
@@ -6956,25 +6963,25 @@
     <row r="71" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D71" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G71" s="3">
         <v>3300002387</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I71" s="3">
         <v>543631083</v>
@@ -6986,25 +6993,25 @@
     <row r="72" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D72" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F72" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G72" s="3">
         <v>3300002298</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I72" s="3">
         <v>490800640</v>
@@ -7016,25 +7023,25 @@
     <row r="73" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D73" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F73" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G73" s="3">
         <v>3300002357</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I73" s="3">
         <v>389023061</v>
@@ -7046,25 +7053,25 @@
     <row r="74" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="G74" s="3">
         <v>3300002351</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I74" s="3">
         <v>623524567</v>
@@ -7156,19 +7163,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2121" r:id="rId77" name="Control 73">
+        <control shapeId="2049" r:id="rId77" name="Control 1">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>73</xdr:row>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>73</xdr:row>
+                <xdr:row>1</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7176,24 +7183,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2121" r:id="rId77" name="Control 73"/>
+        <control shapeId="2049" r:id="rId77" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2120" r:id="rId79" name="Control 72">
+        <control shapeId="2050" r:id="rId79" name="Control 2">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>72</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>72</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7201,24 +7208,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2120" r:id="rId79" name="Control 72"/>
+        <control shapeId="2050" r:id="rId79" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2119" r:id="rId80" name="Control 71">
+        <control shapeId="2051" r:id="rId80" name="Control 3">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>71</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>71</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7226,24 +7233,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2119" r:id="rId80" name="Control 71"/>
+        <control shapeId="2051" r:id="rId80" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2118" r:id="rId81" name="Control 70">
+        <control shapeId="2052" r:id="rId81" name="Control 4">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>70</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>70</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7251,24 +7258,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2118" r:id="rId81" name="Control 70"/>
+        <control shapeId="2052" r:id="rId81" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2117" r:id="rId82" name="Control 69">
+        <control shapeId="2053" r:id="rId82" name="Control 5">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>69</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>69</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7276,24 +7283,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2117" r:id="rId82" name="Control 69"/>
+        <control shapeId="2053" r:id="rId82" name="Control 5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2116" r:id="rId83" name="Control 68">
+        <control shapeId="2054" r:id="rId83" name="Control 6">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>68</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>68</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7301,24 +7308,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2116" r:id="rId83" name="Control 68"/>
+        <control shapeId="2054" r:id="rId83" name="Control 6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2115" r:id="rId84" name="Control 67">
+        <control shapeId="2055" r:id="rId84" name="Control 7">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>67</xdr:row>
+                <xdr:row>7</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>67</xdr:row>
+                <xdr:row>7</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7326,24 +7333,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2115" r:id="rId84" name="Control 67"/>
+        <control shapeId="2055" r:id="rId84" name="Control 7"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2114" r:id="rId85" name="Control 66">
+        <control shapeId="2056" r:id="rId85" name="Control 8">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>66</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>66</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7351,24 +7358,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2114" r:id="rId85" name="Control 66"/>
+        <control shapeId="2056" r:id="rId85" name="Control 8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2113" r:id="rId86" name="Control 65">
+        <control shapeId="2057" r:id="rId86" name="Control 9">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>65</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>65</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7376,24 +7383,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2113" r:id="rId86" name="Control 65"/>
+        <control shapeId="2057" r:id="rId86" name="Control 9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2112" r:id="rId87" name="Control 64">
+        <control shapeId="2058" r:id="rId87" name="Control 10">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>64</xdr:row>
+                <xdr:row>10</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>64</xdr:row>
+                <xdr:row>10</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7401,24 +7408,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2112" r:id="rId87" name="Control 64"/>
+        <control shapeId="2058" r:id="rId87" name="Control 10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2111" r:id="rId88" name="Control 63">
+        <control shapeId="2059" r:id="rId88" name="Control 11">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>63</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>63</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7426,24 +7433,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2111" r:id="rId88" name="Control 63"/>
+        <control shapeId="2059" r:id="rId88" name="Control 11"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2110" r:id="rId89" name="Control 62">
+        <control shapeId="2060" r:id="rId89" name="Control 12">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>62</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>62</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7451,24 +7458,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2110" r:id="rId89" name="Control 62"/>
+        <control shapeId="2060" r:id="rId89" name="Control 12"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2109" r:id="rId90" name="Control 61">
+        <control shapeId="2061" r:id="rId90" name="Control 13">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>61</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>61</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7476,24 +7483,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2109" r:id="rId90" name="Control 61"/>
+        <control shapeId="2061" r:id="rId90" name="Control 13"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2108" r:id="rId91" name="Control 60">
+        <control shapeId="2062" r:id="rId91" name="Control 14">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>60</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>60</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7501,24 +7508,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2108" r:id="rId91" name="Control 60"/>
+        <control shapeId="2062" r:id="rId91" name="Control 14"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2107" r:id="rId92" name="Control 59">
+        <control shapeId="2063" r:id="rId92" name="Control 15">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>59</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>59</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7526,24 +7533,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2107" r:id="rId92" name="Control 59"/>
+        <control shapeId="2063" r:id="rId92" name="Control 15"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2106" r:id="rId93" name="Control 58">
+        <control shapeId="2064" r:id="rId93" name="Control 16">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>58</xdr:row>
+                <xdr:row>16</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>58</xdr:row>
+                <xdr:row>16</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7551,24 +7558,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2106" r:id="rId93" name="Control 58"/>
+        <control shapeId="2064" r:id="rId93" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2105" r:id="rId94" name="Control 57">
+        <control shapeId="2065" r:id="rId94" name="Control 17">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>57</xdr:row>
+                <xdr:row>17</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>57</xdr:row>
+                <xdr:row>17</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7576,24 +7583,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2105" r:id="rId94" name="Control 57"/>
+        <control shapeId="2065" r:id="rId94" name="Control 17"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2104" r:id="rId95" name="Control 56">
+        <control shapeId="2066" r:id="rId95" name="Control 18">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>56</xdr:row>
+                <xdr:row>18</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>56</xdr:row>
+                <xdr:row>18</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7601,24 +7608,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2104" r:id="rId95" name="Control 56"/>
+        <control shapeId="2066" r:id="rId95" name="Control 18"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2103" r:id="rId96" name="Control 55">
+        <control shapeId="2067" r:id="rId96" name="Control 19">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>55</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>55</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7626,24 +7633,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2103" r:id="rId96" name="Control 55"/>
+        <control shapeId="2067" r:id="rId96" name="Control 19"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2102" r:id="rId97" name="Control 54">
+        <control shapeId="2068" r:id="rId97" name="Control 20">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>54</xdr:row>
+                <xdr:row>20</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>54</xdr:row>
+                <xdr:row>20</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7651,24 +7658,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2102" r:id="rId97" name="Control 54"/>
+        <control shapeId="2068" r:id="rId97" name="Control 20"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2101" r:id="rId98" name="Control 53">
+        <control shapeId="2069" r:id="rId98" name="Control 21">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>53</xdr:row>
+                <xdr:row>21</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>53</xdr:row>
+                <xdr:row>21</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7676,24 +7683,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2101" r:id="rId98" name="Control 53"/>
+        <control shapeId="2069" r:id="rId98" name="Control 21"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2100" r:id="rId99" name="Control 52">
+        <control shapeId="2070" r:id="rId99" name="Control 22">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>52</xdr:row>
+                <xdr:row>22</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>52</xdr:row>
+                <xdr:row>22</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7701,24 +7708,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2100" r:id="rId99" name="Control 52"/>
+        <control shapeId="2070" r:id="rId99" name="Control 22"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2099" r:id="rId100" name="Control 51">
+        <control shapeId="2071" r:id="rId100" name="Control 23">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>51</xdr:row>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>51</xdr:row>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7726,24 +7733,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2099" r:id="rId100" name="Control 51"/>
+        <control shapeId="2071" r:id="rId100" name="Control 23"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2098" r:id="rId101" name="Control 50">
+        <control shapeId="2072" r:id="rId101" name="Control 24">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>50</xdr:row>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>50</xdr:row>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7751,24 +7758,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2098" r:id="rId101" name="Control 50"/>
+        <control shapeId="2072" r:id="rId101" name="Control 24"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2097" r:id="rId102" name="Control 49">
+        <control shapeId="2073" r:id="rId102" name="Control 25">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>49</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>49</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7776,24 +7783,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2097" r:id="rId102" name="Control 49"/>
+        <control shapeId="2073" r:id="rId102" name="Control 25"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2096" r:id="rId103" name="Control 48">
+        <control shapeId="2074" r:id="rId103" name="Control 26">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>48</xdr:row>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>48</xdr:row>
+                <xdr:row>26</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7801,24 +7808,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2096" r:id="rId103" name="Control 48"/>
+        <control shapeId="2074" r:id="rId103" name="Control 26"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2095" r:id="rId104" name="Control 47">
+        <control shapeId="2075" r:id="rId104" name="Control 27">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>47</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>47</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7826,24 +7833,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2095" r:id="rId104" name="Control 47"/>
+        <control shapeId="2075" r:id="rId104" name="Control 27"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2094" r:id="rId105" name="Control 46">
+        <control shapeId="2076" r:id="rId105" name="Control 28">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>46</xdr:row>
+                <xdr:row>28</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>46</xdr:row>
+                <xdr:row>28</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7851,24 +7858,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2094" r:id="rId105" name="Control 46"/>
+        <control shapeId="2076" r:id="rId105" name="Control 28"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2093" r:id="rId106" name="Control 45">
+        <control shapeId="2077" r:id="rId106" name="Control 29">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>45</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>45</xdr:row>
+                <xdr:row>29</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7876,24 +7883,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2093" r:id="rId106" name="Control 45"/>
+        <control shapeId="2077" r:id="rId106" name="Control 29"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2092" r:id="rId107" name="Control 44">
+        <control shapeId="2078" r:id="rId107" name="Control 30">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>44</xdr:row>
+                <xdr:row>30</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>44</xdr:row>
+                <xdr:row>30</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7901,24 +7908,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2092" r:id="rId107" name="Control 44"/>
+        <control shapeId="2078" r:id="rId107" name="Control 30"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2091" r:id="rId108" name="Control 43">
+        <control shapeId="2079" r:id="rId108" name="Control 31">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>43</xdr:row>
+                <xdr:row>31</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>43</xdr:row>
+                <xdr:row>31</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7926,24 +7933,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2091" r:id="rId108" name="Control 43"/>
+        <control shapeId="2079" r:id="rId108" name="Control 31"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2090" r:id="rId109" name="Control 42">
+        <control shapeId="2080" r:id="rId109" name="Control 32">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>42</xdr:row>
+                <xdr:row>32</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>42</xdr:row>
+                <xdr:row>32</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7951,24 +7958,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2090" r:id="rId109" name="Control 42"/>
+        <control shapeId="2080" r:id="rId109" name="Control 32"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2089" r:id="rId110" name="Control 41">
+        <control shapeId="2081" r:id="rId110" name="Control 33">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
+                <xdr:row>33</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
+                <xdr:row>33</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -7976,24 +7983,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2089" r:id="rId110" name="Control 41"/>
+        <control shapeId="2081" r:id="rId110" name="Control 33"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2088" r:id="rId111" name="Control 40">
+        <control shapeId="2082" r:id="rId111" name="Control 34">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>34</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>34</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8001,24 +8008,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2088" r:id="rId111" name="Control 40"/>
+        <control shapeId="2082" r:id="rId111" name="Control 34"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2087" r:id="rId112" name="Control 39">
+        <control shapeId="2083" r:id="rId112" name="Control 35">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8026,24 +8033,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2087" r:id="rId112" name="Control 39"/>
+        <control shapeId="2083" r:id="rId112" name="Control 35"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2086" r:id="rId113" name="Control 38">
+        <control shapeId="2084" r:id="rId113" name="Control 36">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
+                <xdr:row>36</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
+                <xdr:row>36</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8051,7 +8058,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2086" r:id="rId113" name="Control 38"/>
+        <control shapeId="2084" r:id="rId113" name="Control 36"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8081,19 +8088,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2084" r:id="rId115" name="Control 36">
+        <control shapeId="2086" r:id="rId115" name="Control 38">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
+                <xdr:row>38</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
+                <xdr:row>38</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8101,24 +8108,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2084" r:id="rId115" name="Control 36"/>
+        <control shapeId="2086" r:id="rId115" name="Control 38"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2083" r:id="rId116" name="Control 35">
+        <control shapeId="2087" r:id="rId116" name="Control 39">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
+                <xdr:row>39</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
+                <xdr:row>39</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8126,24 +8133,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2083" r:id="rId116" name="Control 35"/>
+        <control shapeId="2087" r:id="rId116" name="Control 39"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2082" r:id="rId117" name="Control 34">
+        <control shapeId="2088" r:id="rId117" name="Control 40">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
+                <xdr:row>40</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
+                <xdr:row>40</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8151,24 +8158,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2082" r:id="rId117" name="Control 34"/>
+        <control shapeId="2088" r:id="rId117" name="Control 40"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2081" r:id="rId118" name="Control 33">
+        <control shapeId="2089" r:id="rId118" name="Control 41">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
+                <xdr:row>41</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
+                <xdr:row>41</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8176,24 +8183,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2081" r:id="rId118" name="Control 33"/>
+        <control shapeId="2089" r:id="rId118" name="Control 41"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2080" r:id="rId119" name="Control 32">
+        <control shapeId="2090" r:id="rId119" name="Control 42">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>42</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>42</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8201,24 +8208,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2080" r:id="rId119" name="Control 32"/>
+        <control shapeId="2090" r:id="rId119" name="Control 42"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2079" r:id="rId120" name="Control 31">
+        <control shapeId="2091" r:id="rId120" name="Control 43">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
+                <xdr:row>43</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
+                <xdr:row>43</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8226,24 +8233,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2079" r:id="rId120" name="Control 31"/>
+        <control shapeId="2091" r:id="rId120" name="Control 43"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2078" r:id="rId121" name="Control 30">
+        <control shapeId="2092" r:id="rId121" name="Control 44">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>44</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>44</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8251,24 +8258,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2078" r:id="rId121" name="Control 30"/>
+        <control shapeId="2092" r:id="rId121" name="Control 44"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2077" r:id="rId122" name="Control 29">
+        <control shapeId="2093" r:id="rId122" name="Control 45">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>45</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>45</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8276,24 +8283,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2077" r:id="rId122" name="Control 29"/>
+        <control shapeId="2093" r:id="rId122" name="Control 45"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2076" r:id="rId123" name="Control 28">
+        <control shapeId="2094" r:id="rId123" name="Control 46">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
+                <xdr:row>46</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
+                <xdr:row>46</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8301,24 +8308,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2076" r:id="rId123" name="Control 28"/>
+        <control shapeId="2094" r:id="rId123" name="Control 46"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2075" r:id="rId124" name="Control 27">
+        <control shapeId="2095" r:id="rId124" name="Control 47">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
+                <xdr:row>47</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
+                <xdr:row>47</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8326,24 +8333,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2075" r:id="rId124" name="Control 27"/>
+        <control shapeId="2095" r:id="rId124" name="Control 47"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2074" r:id="rId125" name="Control 26">
+        <control shapeId="2096" r:id="rId125" name="Control 48">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>48</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
+                <xdr:row>48</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8351,24 +8358,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2074" r:id="rId125" name="Control 26"/>
+        <control shapeId="2096" r:id="rId125" name="Control 48"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2073" r:id="rId126" name="Control 25">
+        <control shapeId="2097" r:id="rId126" name="Control 49">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
+                <xdr:row>49</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
+                <xdr:row>49</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8376,24 +8383,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2073" r:id="rId126" name="Control 25"/>
+        <control shapeId="2097" r:id="rId126" name="Control 49"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2072" r:id="rId127" name="Control 24">
+        <control shapeId="2098" r:id="rId127" name="Control 50">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
+                <xdr:row>50</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
+                <xdr:row>50</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8401,24 +8408,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2072" r:id="rId127" name="Control 24"/>
+        <control shapeId="2098" r:id="rId127" name="Control 50"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2071" r:id="rId128" name="Control 23">
+        <control shapeId="2099" r:id="rId128" name="Control 51">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:row>51</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
+                <xdr:row>51</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8426,24 +8433,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2071" r:id="rId128" name="Control 23"/>
+        <control shapeId="2099" r:id="rId128" name="Control 51"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2070" r:id="rId129" name="Control 22">
+        <control shapeId="2100" r:id="rId129" name="Control 52">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
+                <xdr:row>52</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
+                <xdr:row>52</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8451,24 +8458,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2070" r:id="rId129" name="Control 22"/>
+        <control shapeId="2100" r:id="rId129" name="Control 52"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2069" r:id="rId130" name="Control 21">
+        <control shapeId="2101" r:id="rId130" name="Control 53">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>53</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>53</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8476,24 +8483,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2069" r:id="rId130" name="Control 21"/>
+        <control shapeId="2101" r:id="rId130" name="Control 53"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2068" r:id="rId131" name="Control 20">
+        <control shapeId="2102" r:id="rId131" name="Control 54">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
+                <xdr:row>54</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
+                <xdr:row>54</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8501,24 +8508,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2068" r:id="rId131" name="Control 20"/>
+        <control shapeId="2102" r:id="rId131" name="Control 54"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2067" r:id="rId132" name="Control 19">
+        <control shapeId="2103" r:id="rId132" name="Control 55">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
+                <xdr:row>55</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
+                <xdr:row>55</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8526,24 +8533,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2067" r:id="rId132" name="Control 19"/>
+        <control shapeId="2103" r:id="rId132" name="Control 55"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2066" r:id="rId133" name="Control 18">
+        <control shapeId="2104" r:id="rId133" name="Control 56">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
+                <xdr:row>56</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
+                <xdr:row>56</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8551,24 +8558,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2066" r:id="rId133" name="Control 18"/>
+        <control shapeId="2104" r:id="rId133" name="Control 56"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2065" r:id="rId134" name="Control 17">
+        <control shapeId="2105" r:id="rId134" name="Control 57">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>57</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>57</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8576,24 +8583,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2065" r:id="rId134" name="Control 17"/>
+        <control shapeId="2105" r:id="rId134" name="Control 57"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2064" r:id="rId135" name="Control 16">
+        <control shapeId="2106" r:id="rId135" name="Control 58">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
+                <xdr:row>58</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
+                <xdr:row>58</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8601,24 +8608,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2064" r:id="rId135" name="Control 16"/>
+        <control shapeId="2106" r:id="rId135" name="Control 58"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2063" r:id="rId136" name="Control 15">
+        <control shapeId="2107" r:id="rId136" name="Control 59">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>59</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>59</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8626,24 +8633,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2063" r:id="rId136" name="Control 15"/>
+        <control shapeId="2107" r:id="rId136" name="Control 59"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2062" r:id="rId137" name="Control 14">
+        <control shapeId="2108" r:id="rId137" name="Control 60">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
+                <xdr:row>60</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
+                <xdr:row>60</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8651,24 +8658,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2062" r:id="rId137" name="Control 14"/>
+        <control shapeId="2108" r:id="rId137" name="Control 60"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2061" r:id="rId138" name="Control 13">
+        <control shapeId="2109" r:id="rId138" name="Control 61">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>61</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>61</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8676,24 +8683,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2061" r:id="rId138" name="Control 13"/>
+        <control shapeId="2109" r:id="rId138" name="Control 61"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2060" r:id="rId139" name="Control 12">
+        <control shapeId="2110" r:id="rId139" name="Control 62">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>62</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>62</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8701,24 +8708,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2060" r:id="rId139" name="Control 12"/>
+        <control shapeId="2110" r:id="rId139" name="Control 62"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2059" r:id="rId140" name="Control 11">
+        <control shapeId="2111" r:id="rId140" name="Control 63">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>63</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>63</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8726,24 +8733,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2059" r:id="rId140" name="Control 11"/>
+        <control shapeId="2111" r:id="rId140" name="Control 63"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2058" r:id="rId141" name="Control 10">
+        <control shapeId="2112" r:id="rId141" name="Control 64">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>64</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>64</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8751,24 +8758,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2058" r:id="rId141" name="Control 10"/>
+        <control shapeId="2112" r:id="rId141" name="Control 64"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId142" name="Control 9">
+        <control shapeId="2113" r:id="rId142" name="Control 65">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>65</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>65</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8776,24 +8783,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2057" r:id="rId142" name="Control 9"/>
+        <control shapeId="2113" r:id="rId142" name="Control 65"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId143" name="Control 8">
+        <control shapeId="2114" r:id="rId143" name="Control 66">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>66</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>66</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8801,24 +8808,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2056" r:id="rId143" name="Control 8"/>
+        <control shapeId="2114" r:id="rId143" name="Control 66"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId144" name="Control 7">
+        <control shapeId="2115" r:id="rId144" name="Control 67">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>67</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>67</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8826,24 +8833,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2055" r:id="rId144" name="Control 7"/>
+        <control shapeId="2115" r:id="rId144" name="Control 67"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2054" r:id="rId145" name="Control 6">
+        <control shapeId="2116" r:id="rId145" name="Control 68">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>68</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>68</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8851,24 +8858,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2054" r:id="rId145" name="Control 6"/>
+        <control shapeId="2116" r:id="rId145" name="Control 68"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2053" r:id="rId146" name="Control 5">
+        <control shapeId="2117" r:id="rId146" name="Control 69">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>69</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>69</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8876,24 +8883,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2053" r:id="rId146" name="Control 5"/>
+        <control shapeId="2117" r:id="rId146" name="Control 69"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId147" name="Control 4">
+        <control shapeId="2118" r:id="rId147" name="Control 70">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>70</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>70</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8901,24 +8908,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId147" name="Control 4"/>
+        <control shapeId="2118" r:id="rId147" name="Control 70"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId148" name="Control 3">
+        <control shapeId="2119" r:id="rId148" name="Control 71">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>71</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>71</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8926,24 +8933,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2051" r:id="rId148" name="Control 3"/>
+        <control shapeId="2119" r:id="rId148" name="Control 71"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2050" r:id="rId149" name="Control 2">
+        <control shapeId="2120" r:id="rId149" name="Control 72">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>72</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>72</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8951,24 +8958,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2050" r:id="rId149" name="Control 2"/>
+        <control shapeId="2120" r:id="rId149" name="Control 72"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId150" name="Control 1">
+        <control shapeId="2121" r:id="rId150" name="Control 73">
           <controlPr defaultSize="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:row>73</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:row>73</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -8976,7 +8983,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId150" name="Control 1"/>
+        <control shapeId="2121" r:id="rId150" name="Control 73"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>